<commit_message>
Adding entry_date to reported stocks instead of reported date
</commit_message>
<xml_diff>
--- a/data/Trade_List_2017_Present.xlsx
+++ b/data/Trade_List_2017_Present.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newco\Documents\Repos\Python\Upwork\Steven\EarningsReversalPattern\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47AABF6F-5ADA-40B3-96AC-B7EA36E9D903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65769322-2434-4E0F-91A7-435E84B6940B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5730" yWindow="-21720" windowWidth="38640" windowHeight="21840"/>
+    <workbookView xWindow="19560" yWindow="-20610" windowWidth="33390" windowHeight="19785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trades List" sheetId="1" r:id="rId1"/>
@@ -2113,7 +2113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.00%;\-#,##0.00%"/>
@@ -2136,7 +2136,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2147,6 +2147,18 @@
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
         <bgColor indexed="16"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2171,7 +2183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2191,6 +2203,29 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2572,21 +2607,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U971"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A917" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C942" sqref="C942"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" style="2" customWidth="1"/>
@@ -63897,263 +63932,263 @@
         <v>381.63</v>
       </c>
     </row>
-    <row r="944" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A944" s="1">
+    <row r="944" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A944" s="7">
         <v>396</v>
       </c>
-      <c r="B944" s="1" t="s">
+      <c r="B944" s="7" t="s">
         <v>668</v>
       </c>
-      <c r="C944" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D944" s="1" t="s">
+      <c r="C944" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D944" s="7" t="s">
         <v>684</v>
       </c>
-      <c r="E944" s="1" t="s">
+      <c r="E944" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F944" s="5">
+      <c r="F944" s="8">
         <v>325.16000000000003</v>
       </c>
-      <c r="G944" s="2">
+      <c r="G944" s="9">
         <v>31</v>
       </c>
-      <c r="H944" s="5">
-        <v>0</v>
-      </c>
-      <c r="I944" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J944" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K944" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L944" s="1" t="s">
+      <c r="H944" s="8">
+        <v>0</v>
+      </c>
+      <c r="I944" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J944" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K944" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L944" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M944" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N944" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O944" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P944" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q944" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R944" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S944" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T944" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="U944" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="945" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A945" s="1">
+      <c r="M944" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="N944" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="O944" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="P944" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q944" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="R944" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="S944" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="T944" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="U944" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="945" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A945" s="11">
         <v>396</v>
       </c>
-      <c r="B945" s="1" t="s">
+      <c r="B945" s="11" t="s">
         <v>685</v>
       </c>
-      <c r="C945" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D945" s="1" t="s">
+      <c r="C945" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D945" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="E945" s="1" t="s">
+      <c r="E945" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F945" s="5">
+      <c r="F945" s="12">
         <v>351.18</v>
       </c>
-      <c r="G945" s="2">
+      <c r="G945" s="13">
         <v>16</v>
       </c>
-      <c r="H945" s="5">
-        <v>0</v>
-      </c>
-      <c r="I945" s="5">
+      <c r="H945" s="12">
+        <v>0</v>
+      </c>
+      <c r="I945" s="12">
         <v>416.32</v>
       </c>
-      <c r="J945" s="6">
+      <c r="J945" s="14">
         <v>0.08</v>
       </c>
-      <c r="K945" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L945" s="1" t="s">
+      <c r="K945" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L945" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="M945" s="6">
+      <c r="M945" s="14">
         <v>0.93870000000000009</v>
       </c>
-      <c r="N945" s="6">
+      <c r="N945" s="14">
         <v>0.93870000000000009</v>
       </c>
-      <c r="O945" s="6">
+      <c r="O945" s="14">
         <v>1</v>
       </c>
-      <c r="P945" s="5">
+      <c r="P945" s="12">
         <v>-27.2</v>
       </c>
-      <c r="Q945" s="6">
+      <c r="Q945" s="14">
         <v>-5.1999999999999998E-3</v>
       </c>
-      <c r="R945" s="5">
+      <c r="R945" s="12">
         <v>416.32</v>
       </c>
-      <c r="S945" s="6">
+      <c r="S945" s="14">
         <v>0.08</v>
       </c>
-      <c r="T945" s="5">
+      <c r="T945" s="12">
         <v>351.18</v>
       </c>
-      <c r="U945" s="5">
+      <c r="U945" s="12">
         <v>323.45999999999998</v>
       </c>
     </row>
-    <row r="946" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A946" s="1">
+    <row r="946" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A946" s="11">
         <v>396</v>
       </c>
-      <c r="B946" s="1" t="s">
+      <c r="B946" s="11" t="s">
         <v>673</v>
       </c>
-      <c r="C946" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D946" s="1" t="s">
+      <c r="C946" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D946" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="E946" s="1" t="s">
+      <c r="E946" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F946" s="5">
+      <c r="F946" s="12">
         <v>328.78</v>
       </c>
-      <c r="G946" s="2">
+      <c r="G946" s="13">
         <v>15</v>
       </c>
-      <c r="H946" s="5">
-        <v>0</v>
-      </c>
-      <c r="I946" s="5">
+      <c r="H946" s="12">
+        <v>0</v>
+      </c>
+      <c r="I946" s="12">
         <v>54.3</v>
       </c>
-      <c r="J946" s="6">
+      <c r="J946" s="14">
         <v>1.11E-2</v>
       </c>
-      <c r="K946" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L946" s="1" t="s">
+      <c r="K946" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L946" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="M946" s="6">
+      <c r="M946" s="14">
         <v>0.13059999999999999</v>
       </c>
-      <c r="N946" s="6">
+      <c r="N946" s="14">
         <v>0.93870000000000009</v>
       </c>
-      <c r="O946" s="6">
+      <c r="O946" s="14">
         <v>0.19190000000000002</v>
       </c>
-      <c r="P946" s="5">
+      <c r="P946" s="12">
         <v>-25.5</v>
       </c>
-      <c r="Q946" s="6">
+      <c r="Q946" s="14">
         <v>-5.1999999999999998E-3</v>
       </c>
-      <c r="R946" s="5">
+      <c r="R946" s="12">
         <v>390.3</v>
       </c>
-      <c r="S946" s="6">
+      <c r="S946" s="14">
         <v>0.08</v>
       </c>
-      <c r="T946" s="5">
+      <c r="T946" s="12">
         <v>351.18</v>
       </c>
-      <c r="U946" s="5">
+      <c r="U946" s="12">
         <v>323.45999999999998</v>
       </c>
     </row>
-    <row r="947" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A947" s="1">
+    <row r="947" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A947" s="11">
         <v>397</v>
       </c>
-      <c r="B947" s="1" t="s">
+      <c r="B947" s="11" t="s">
         <v>668</v>
       </c>
-      <c r="C947" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D947" s="1" t="s">
+      <c r="C947" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D947" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E947" s="1" t="s">
+      <c r="E947" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F947" s="5">
+      <c r="F947" s="12">
         <v>284.07</v>
       </c>
-      <c r="G947" s="2">
+      <c r="G947" s="13">
         <v>36</v>
       </c>
-      <c r="H947" s="5">
-        <v>0</v>
-      </c>
-      <c r="I947" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J947" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K947" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L947" s="1" t="s">
+      <c r="H947" s="12">
+        <v>0</v>
+      </c>
+      <c r="I947" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J947" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K947" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L947" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M947" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N947" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O947" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P947" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q947" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R947" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S947" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T947" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="U947" s="2" t="s">
+      <c r="M947" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N947" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O947" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P947" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q947" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="R947" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="S947" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="T947" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="U947" s="13" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>